<commit_message>
add the new file.
</commit_message>
<xml_diff>
--- a/count.xlsx
+++ b/count.xlsx
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:Q31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -722,15 +722,14 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B8" s="1">
-        <f>3000000</f>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" s="1">
         <f>(1-(D8*0.06)/(1+D8*0.06))*B8</f>
-        <v>2830188.6792452829</v>
+        <v>2830188679.2452831</v>
       </c>
       <c r="F8" t="str">
         <f>(1-(D8*0.06)/(1+D8*0.06))*100&amp;"%"</f>
@@ -758,14 +757,14 @@
     <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B9" s="1">
         <f>B8</f>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" ref="E9:E72" si="0">(1-(D9*0.06)/(1+D9*0.06))*B9</f>
-        <v>2678571.4285714286</v>
+        <v>2678571428.5714288</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" ref="F9:F36" si="1">(1-(D9*0.06)/(1+D9*0.06))*100&amp;"%"</f>
@@ -793,14 +792,14 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B10" s="1">
         <f t="shared" ref="B10:B73" si="2">B9</f>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>2542372.881355932</v>
+        <v>2542372881.3559322</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -828,14 +827,14 @@
     <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B11" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>2419354.8387096771</v>
+        <v>2419354838.7096772</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -863,14 +862,14 @@
     <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B12" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>2307692.307692308</v>
+        <v>2307692307.6923079</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -898,14 +897,14 @@
     <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B13" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D13">
         <v>6</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>2205882.3529411769</v>
+        <v>2205882352.9411764</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
@@ -936,14 +935,14 @@
     <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B14" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D14">
         <v>7</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>2112676.0563380281</v>
+        <v>2112676056.338028</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
@@ -974,14 +973,14 @@
     <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B15" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D15">
         <v>8</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>2027027.027027027</v>
+        <v>2027027027.0270269</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -991,14 +990,14 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B16" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D16">
         <v>9</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>1948051.9480519481</v>
+        <v>1948051948.0519481</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
@@ -1026,14 +1025,14 @@
     <row r="17" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B17" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>1875000</v>
+        <v>1875000000</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
@@ -1061,14 +1060,14 @@
     <row r="18" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B18" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D18">
         <v>20</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>1363636.3636363638</v>
+        <v>1363636363.6363637</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
@@ -1078,14 +1077,14 @@
     <row r="19" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D19">
         <v>30</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>1071428.5714285716</v>
+        <v>1071428571.4285716</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
@@ -1095,14 +1094,14 @@
     <row r="20" spans="2:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D20">
         <v>40</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>882352.94117647049</v>
+        <v>882352941.1764704</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
@@ -1112,14 +1111,14 @@
     <row r="21" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B21" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D21">
         <v>50</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>750000</v>
+        <v>750000000</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
@@ -1129,14 +1128,14 @@
     <row r="22" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B22" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D22">
         <v>60</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>652173.91304347815</v>
+        <v>652173913.04347813</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
@@ -1146,14 +1145,14 @@
     <row r="23" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B23" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D23">
         <v>70</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>576923.07692307688</v>
+        <v>576923076.92307687</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
@@ -1163,14 +1162,14 @@
     <row r="24" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B24" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D24">
         <v>80</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>517241.37931034487</v>
+        <v>517241379.31034487</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
@@ -1180,14 +1179,14 @@
     <row r="25" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B25" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D25">
         <v>90</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>468750</v>
+        <v>468750000</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="1"/>
@@ -1197,14 +1196,14 @@
     <row r="26" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B26" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D26">
         <v>100</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>428571.4285714287</v>
+        <v>428571428.57142872</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
@@ -1214,14 +1213,14 @@
     <row r="27" spans="2:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D27">
         <v>200</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>230769.23076923061</v>
+        <v>230769230.7692306</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="1"/>
@@ -1237,14 +1236,14 @@
     <row r="28" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B28" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D28">
         <v>300</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>157894.73684210543</v>
+        <v>157894736.84210542</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="1"/>
@@ -1270,14 +1269,14 @@
     <row r="29" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B29" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D29">
         <v>400</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>120000.0000000001</v>
+        <v>120000000.0000001</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="1"/>
@@ -1299,14 +1298,14 @@
     <row r="30" spans="2:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D30">
         <v>500</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>96774.193548387004</v>
+        <v>96774193.548387006</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="1"/>
@@ -1328,14 +1327,14 @@
     <row r="31" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B31" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D31">
         <v>600</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>81081.08108108092</v>
+        <v>81081081.081080914</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="1"/>
@@ -1351,14 +1350,14 @@
     <row r="32" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B32" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D32">
         <v>700</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>69767.441860465246</v>
+        <v>69767441.860465243</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
@@ -1374,14 +1373,14 @@
     <row r="33" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B33" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D33">
         <v>800</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>61224.489795918438</v>
+        <v>61224489.795918435</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="1"/>
@@ -1410,14 +1409,14 @@
     <row r="34" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B34" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D34">
         <v>900</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>54545.454545454566</v>
+        <v>54545454.545454562</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
@@ -1446,14 +1445,14 @@
     <row r="35" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B35" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D35">
         <v>1000</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>49180.327868852517</v>
+        <v>49180327.868852511</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
@@ -1475,14 +1474,14 @@
     <row r="36" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B36" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D36">
         <v>1500</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" si="0"/>
-        <v>32967.03296703285</v>
+        <v>32967032.96703285</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
@@ -1510,14 +1509,14 @@
     <row r="37" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B37" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D37">
         <v>2000</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="0"/>
-        <v>24793.388429751983</v>
+        <v>24793388.429751985</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" ref="F37:F54" si="3">(1-(D37*0.06)/(1+D37*0.06))*100&amp;"%"</f>
@@ -1545,14 +1544,14 @@
     <row r="38" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B38" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D38">
         <v>2500</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="0"/>
-        <v>19867.549668874275</v>
+        <v>19867549.668874275</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="3"/>
@@ -1574,14 +1573,14 @@
     <row r="39" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B39" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D39">
         <v>3000</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" si="0"/>
-        <v>16574.585635359075</v>
+        <v>16574585.635359073</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="3"/>
@@ -1605,14 +1604,14 @@
     <row r="40" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B40" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D40">
         <v>3500</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" si="0"/>
-        <v>14218.009478673133</v>
+        <v>14218009.478673132</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="3"/>
@@ -1636,14 +1635,14 @@
     <row r="41" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B41" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D41">
         <v>4000</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="0"/>
-        <v>12448.132780082944</v>
+        <v>12448132.780082943</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="3"/>
@@ -1653,14 +1652,14 @@
     <row r="42" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B42" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D42">
         <v>4500</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" si="0"/>
-        <v>11070.110701106862</v>
+        <v>11070110.701106861</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="3"/>
@@ -1682,14 +1681,14 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B43" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D43">
         <v>5000</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" si="0"/>
-        <v>9966.7774086379395</v>
+        <v>9966777.408637939</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="3"/>
@@ -1711,14 +1710,14 @@
     <row r="44" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B44" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D44">
         <v>5500</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="0"/>
-        <v>9063.444108761254</v>
+        <v>9063444.1087612547</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="3"/>
@@ -1728,14 +1727,14 @@
     <row r="45" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B45" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D45">
         <v>6000</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="0"/>
-        <v>8310.2493074791455</v>
+        <v>8310249.307479145</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="3"/>
@@ -1745,14 +1744,14 @@
     <row r="46" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B46" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D46">
         <v>6500</v>
       </c>
       <c r="E46" s="1">
         <f t="shared" si="0"/>
-        <v>7672.6342710998761</v>
+        <v>7672634.2710998766</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="3"/>
@@ -1762,14 +1761,14 @@
     <row r="47" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B47" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D47">
         <v>7000</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" si="0"/>
-        <v>7125.8907363420667</v>
+        <v>7125890.7363420669</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="3"/>
@@ -1779,14 +1778,14 @@
     <row r="48" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B48" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D48">
         <v>7500</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" si="0"/>
-        <v>6651.884700665134</v>
+        <v>6651884.700665134</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="3"/>
@@ -1796,14 +1795,14 @@
     <row r="49" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B49" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D49">
         <v>8000</v>
       </c>
       <c r="E49" s="1">
         <f t="shared" si="0"/>
-        <v>6237.0062370060705</v>
+        <v>6237006.237006071</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="3"/>
@@ -1813,14 +1812,14 @@
     <row r="50" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B50" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D50">
         <v>8500</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" si="0"/>
-        <v>5870.8414872800095</v>
+        <v>5870841.4872800093</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="3"/>
@@ -1830,14 +1829,14 @@
     <row r="51" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B51" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D51">
         <v>9000</v>
       </c>
       <c r="E51" s="1">
         <f t="shared" si="0"/>
-        <v>5545.2865064695707</v>
+        <v>5545286.506469571</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="3"/>
@@ -1847,14 +1846,14 @@
     <row r="52" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B52" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D52">
         <v>9500</v>
       </c>
       <c r="E52" s="1">
         <f t="shared" si="0"/>
-        <v>5253.9404553414433</v>
+        <v>5253940.4553414434</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="3"/>
@@ -1864,14 +1863,14 @@
     <row r="53" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B53" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D53">
         <v>10000</v>
       </c>
       <c r="E53" s="1">
         <f t="shared" si="0"/>
-        <v>4991.6805324459192</v>
+        <v>4991680.5324459188</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="3"/>
@@ -1881,14 +1880,14 @@
     <row r="54" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B54" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D54">
         <v>11000</v>
       </c>
       <c r="E54" s="1">
         <f t="shared" si="0"/>
-        <v>4538.5779122542044</v>
+        <v>4538577.912254205</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="3"/>
@@ -1898,14 +1897,14 @@
     <row r="55" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B55" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D55">
         <v>12000</v>
       </c>
       <c r="E55" s="1">
         <f t="shared" si="0"/>
-        <v>4160.8876560332856</v>
+        <v>4160887.6560332854</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" ref="F55:F66" si="4">(1-(D55*0.06)/(1+D55*0.06))*100&amp;"%"</f>
@@ -1915,14 +1914,14 @@
     <row r="56" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B56" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D56">
         <v>13000</v>
       </c>
       <c r="E56" s="1">
         <f t="shared" si="0"/>
-        <v>3841.2291933419551</v>
+        <v>3841229.1933419551</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="4"/>
@@ -1932,14 +1931,14 @@
     <row r="57" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B57" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D57">
         <v>14000</v>
       </c>
       <c r="E57" s="1">
         <f t="shared" si="0"/>
-        <v>3567.181926278362</v>
+        <v>3567181.9262783621</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="4"/>
@@ -1949,14 +1948,14 @@
     <row r="58" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B58" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D58">
         <v>15000</v>
       </c>
       <c r="E58" s="1">
         <f t="shared" si="0"/>
-        <v>3329.6337402886065</v>
+        <v>3329633.7402886068</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="4"/>
@@ -1966,14 +1965,14 @@
     <row r="59" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B59" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D59">
         <v>16000</v>
       </c>
       <c r="E59" s="1">
         <f t="shared" si="0"/>
-        <v>3121.748178980366</v>
+        <v>3121748.1789803659</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="4"/>
@@ -1983,14 +1982,14 @@
     <row r="60" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B60" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D60">
         <v>17000</v>
       </c>
       <c r="E60" s="1">
         <f t="shared" si="0"/>
-        <v>2938.2957884427351</v>
+        <v>2938295.7884427351</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="4"/>
@@ -2000,14 +1999,14 @@
     <row r="61" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B61" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D61">
         <v>18000</v>
       </c>
       <c r="E61" s="1">
         <f t="shared" si="0"/>
-        <v>2775.2081406106076</v>
+        <v>2775208.1406106078</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="4"/>
@@ -2017,14 +2016,14 @@
     <row r="62" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B62" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D62">
         <v>19000</v>
       </c>
       <c r="E62" s="1">
         <f t="shared" si="0"/>
-        <v>2629.272567923002</v>
+        <v>2629272.5679230024</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="4"/>
@@ -2034,14 +2033,14 @@
     <row r="63" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B63" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D63">
         <v>20000</v>
       </c>
       <c r="E63" s="1">
         <f t="shared" si="0"/>
-        <v>2497.9184013322888</v>
+        <v>2497918.4013322885</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="4"/>
@@ -2051,14 +2050,14 @@
     <row r="64" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B64" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D64">
         <v>21000</v>
       </c>
       <c r="E64" s="1">
         <f t="shared" si="0"/>
-        <v>2379.0642347343291</v>
+        <v>2379064.2347343294</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="4"/>
@@ -2068,14 +2067,14 @@
     <row r="65" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B65" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D65">
         <v>22000</v>
       </c>
       <c r="E65" s="1">
         <f t="shared" si="0"/>
-        <v>2271.0068130205041</v>
+        <v>2271006.8130205041</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="4"/>
@@ -2085,14 +2084,14 @@
     <row r="66" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B66" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D66">
         <v>23000</v>
       </c>
       <c r="E66" s="1">
         <f t="shared" si="0"/>
-        <v>2172.3388848660097</v>
+        <v>2172338.8848660095</v>
       </c>
       <c r="F66" t="str">
         <f t="shared" si="4"/>
@@ -2102,14 +2101,14 @@
     <row r="67" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B67" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D67">
         <v>24000</v>
       </c>
       <c r="E67" s="1">
         <f t="shared" si="0"/>
-        <v>2081.8875780708181</v>
+        <v>2081887.578070818</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" ref="F67:F74" si="5">(1-(D67*0.06)/(1+D67*0.06))*100&amp;"%"</f>
@@ -2119,14 +2118,14 @@
     <row r="68" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B68" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D68">
         <v>25000</v>
       </c>
       <c r="E68" s="1">
         <f t="shared" si="0"/>
-        <v>1998.6675549634735</v>
+        <v>1998667.5549634737</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="5"/>
@@ -2136,14 +2135,14 @@
     <row r="69" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B69" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D69">
         <v>26000</v>
       </c>
       <c r="E69" s="1">
         <f t="shared" si="0"/>
-        <v>1921.8449711724261</v>
+        <v>1921844.9711724261</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="5"/>
@@ -2153,14 +2152,14 @@
     <row r="70" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B70" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D70">
         <v>27000</v>
       </c>
       <c r="E70" s="1">
         <f t="shared" si="0"/>
-        <v>1850.7094386179813</v>
+        <v>1850709.4386179813</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="5"/>
@@ -2170,14 +2169,14 @@
     <row r="71" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B71" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D71">
         <v>28000</v>
       </c>
       <c r="E71" s="1">
         <f t="shared" si="0"/>
-        <v>1784.6519928612636</v>
+        <v>1784651.9928612637</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="5"/>
@@ -2187,14 +2186,14 @@
     <row r="72" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B72" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D72">
         <v>29000</v>
       </c>
       <c r="E72" s="1">
         <f t="shared" si="0"/>
-        <v>1723.1476163125369</v>
+        <v>1723147.6163125369</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="5"/>
@@ -2204,14 +2203,14 @@
     <row r="73" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B73" s="1">
         <f t="shared" si="2"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D73">
         <v>30000</v>
       </c>
       <c r="E73" s="1">
         <f t="shared" ref="E73:E108" si="6">(1-(D73*0.06)/(1+D73*0.06))*B73</f>
-        <v>1665.7412548584105</v>
+        <v>1665741.2548584105</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="5"/>
@@ -2221,14 +2220,14 @@
     <row r="74" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B74" s="1">
         <f t="shared" ref="B74:B108" si="7">B73</f>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D74">
         <v>32000</v>
       </c>
       <c r="E74" s="1">
         <f t="shared" si="6"/>
-        <v>1561.6866215513169</v>
+        <v>1561686.6215513169</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="5"/>
@@ -2238,14 +2237,14 @@
     <row r="75" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B75" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D75">
         <v>34000</v>
       </c>
       <c r="E75" s="1">
         <f t="shared" si="6"/>
-        <v>1469.8677119058257</v>
+        <v>1469867.7119058257</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" ref="F75:F108" si="8">(1-(D75*0.06)/(1+D75*0.06))*100&amp;"%"</f>
@@ -2255,14 +2254,14 @@
     <row r="76" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B76" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D76">
         <v>36000</v>
       </c>
       <c r="E76" s="1">
         <f t="shared" si="6"/>
-        <v>1388.2461823230274</v>
+        <v>1388246.1823230274</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="8"/>
@@ -2272,14 +2271,14 @@
     <row r="77" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B77" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D77">
         <v>38000</v>
       </c>
       <c r="E77" s="1">
         <f t="shared" si="6"/>
-        <v>1315.2126260410623</v>
+        <v>1315212.6260410624</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="8"/>
@@ -2289,14 +2288,14 @@
     <row r="78" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B78" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D78">
         <v>40000</v>
       </c>
       <c r="E78" s="1">
         <f t="shared" si="6"/>
-        <v>1249.4793835902128</v>
+        <v>1249479.383590213</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="8"/>
@@ -2306,14 +2305,14 @@
     <row r="79" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B79" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D79">
         <v>42000</v>
       </c>
       <c r="E79" s="1">
         <f t="shared" si="6"/>
-        <v>1190.0039666797868</v>
+        <v>1190003.9666797868</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="8"/>
@@ -2323,14 +2322,14 @@
     <row r="80" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B80" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D80">
         <v>44000</v>
       </c>
       <c r="E80" s="1">
         <f t="shared" si="6"/>
-        <v>1135.9333585762022</v>
+        <v>1135933.3585762021</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="8"/>
@@ -2340,14 +2339,14 @@
     <row r="81" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B81" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D81">
         <v>46000</v>
       </c>
       <c r="E81" s="1">
         <f t="shared" si="6"/>
-        <v>1086.5628395508863</v>
+        <v>1086562.8395508863</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="8"/>
@@ -2357,14 +2356,14 @@
     <row r="82" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B82" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D82">
         <v>48000</v>
       </c>
       <c r="E82" s="1">
         <f t="shared" si="6"/>
-        <v>1041.3051023949738</v>
+        <v>1041305.1023949737</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="8"/>
@@ -2374,14 +2373,14 @@
     <row r="83" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B83" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D83">
         <v>50000</v>
       </c>
       <c r="E83" s="1">
         <f t="shared" si="6"/>
-        <v>999.66677774077084</v>
+        <v>999666.77774077083</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="8"/>
@@ -2391,14 +2390,14 @@
     <row r="84" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B84" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D84">
         <v>52000</v>
       </c>
       <c r="E84" s="1">
         <f t="shared" si="6"/>
-        <v>961.23037487993997</v>
+        <v>961230.37487994006</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="8"/>
@@ -2408,14 +2407,14 @@
     <row r="85" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B85" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D85">
         <v>54000</v>
       </c>
       <c r="E85" s="1">
         <f t="shared" si="6"/>
-        <v>925.64023449548392</v>
+        <v>925640.23449548392</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="8"/>
@@ -2425,14 +2424,14 @@
     <row r="86" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B86" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D86">
         <v>56000</v>
       </c>
       <c r="E86" s="1">
         <f t="shared" si="6"/>
-        <v>892.59149062792528</v>
+        <v>892591.49062792526</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="8"/>
@@ -2442,14 +2441,14 @@
     <row r="87" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B87" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D87">
         <v>58000</v>
       </c>
       <c r="E87" s="1">
         <f t="shared" si="6"/>
-        <v>861.82131571388436</v>
+        <v>861821.31571388431</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="8"/>
@@ -2459,14 +2458,14 @@
     <row r="88" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B88" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D88">
         <v>60000</v>
       </c>
       <c r="E88" s="1">
         <f t="shared" si="6"/>
-        <v>833.10191613439338</v>
+        <v>833101.91613439331</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="8"/>
@@ -2476,14 +2475,14 @@
     <row r="89" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B89" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D89">
         <v>62000</v>
       </c>
       <c r="E89" s="1">
         <f t="shared" si="6"/>
-        <v>806.2348830960575</v>
+        <v>806234.88309605746</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="8"/>
@@ -2493,14 +2492,14 @@
     <row r="90" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B90" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D90">
         <v>64000</v>
       </c>
       <c r="E90" s="1">
         <f t="shared" si="6"/>
-        <v>781.04660244715524</v>
+        <v>781046.60244715516</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="8"/>
@@ -2510,14 +2509,14 @@
     <row r="91" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B91" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D91">
         <v>66000</v>
       </c>
       <c r="E91" s="1">
         <f t="shared" si="6"/>
-        <v>757.3844988639778</v>
+        <v>757384.49886397773</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="8"/>
@@ -2527,14 +2526,14 @@
     <row r="92" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B92" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D92">
         <v>68000</v>
       </c>
       <c r="E92" s="1">
         <f t="shared" si="6"/>
-        <v>735.11394266112529</v>
+        <v>735113.94266112533</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="8"/>
@@ -2544,14 +2543,14 @@
     <row r="93" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B93" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D93">
         <v>70000</v>
       </c>
       <c r="E93" s="1">
         <f t="shared" si="6"/>
-        <v>714.11568674140108</v>
+        <v>714115.68674140109</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" si="8"/>
@@ -2561,14 +2560,14 @@
     <row r="94" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B94" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D94">
         <v>72000</v>
       </c>
       <c r="E94" s="1">
         <f t="shared" si="6"/>
-        <v>694.28373061775073</v>
+        <v>694283.73061775079</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" si="8"/>
@@ -2578,14 +2577,14 @@
     <row r="95" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B95" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D95">
         <v>74000</v>
       </c>
       <c r="E95" s="1">
         <f t="shared" si="6"/>
-        <v>675.52353073618838</v>
+        <v>675523.5307361884</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" si="8"/>
@@ -2595,14 +2594,14 @@
     <row r="96" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B96" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D96">
         <v>76000</v>
       </c>
       <c r="E96" s="1">
         <f t="shared" si="6"/>
-        <v>657.75049331273647</v>
+        <v>657750.49331273651</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" si="8"/>
@@ -2612,14 +2611,14 @@
     <row r="97" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B97" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D97">
         <v>78000</v>
       </c>
       <c r="E97" s="1">
         <f t="shared" si="6"/>
-        <v>640.88869899592282</v>
+        <v>640888.69899592281</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" si="8"/>
@@ -2629,14 +2628,14 @@
     <row r="98" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B98" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D98">
         <v>80000</v>
       </c>
       <c r="E98" s="1">
         <f t="shared" si="6"/>
-        <v>624.86981878762117</v>
+        <v>624869.8187876211</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="8"/>
@@ -2646,14 +2645,14 @@
     <row r="99" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B99" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D99">
         <v>82000</v>
       </c>
       <c r="E99" s="1">
         <f t="shared" si="6"/>
-        <v>609.63218857967854</v>
+        <v>609632.18857967854</v>
       </c>
       <c r="F99" t="str">
         <f t="shared" si="8"/>
@@ -2663,14 +2662,14 @@
     <row r="100" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B100" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D100">
         <v>84000</v>
       </c>
       <c r="E100" s="1">
         <f t="shared" si="6"/>
-        <v>595.12001586981</v>
+        <v>595120.01586981001</v>
       </c>
       <c r="F100" t="str">
         <f t="shared" si="8"/>
@@ -2680,14 +2679,14 @@
     <row r="101" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B101" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D101">
         <v>86000</v>
       </c>
       <c r="E101" s="1">
         <f t="shared" si="6"/>
-        <v>581.28269715163049</v>
+        <v>581282.69715163053</v>
       </c>
       <c r="F101" t="str">
         <f t="shared" si="8"/>
@@ -2697,14 +2696,14 @@
     <row r="102" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B102" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D102">
         <v>88000</v>
       </c>
       <c r="E102" s="1">
         <f t="shared" si="6"/>
-        <v>568.07422836591127</v>
+        <v>568074.22836591129</v>
       </c>
       <c r="F102" t="str">
         <f t="shared" si="8"/>
@@ -2714,14 +2713,14 @@
     <row r="103" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B103" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D103">
         <v>90000</v>
       </c>
       <c r="E103" s="1">
         <f t="shared" si="6"/>
-        <v>555.45269394563502</v>
+        <v>555452.69394563499</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="8"/>
@@ -2731,14 +2730,14 @@
     <row r="104" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B104" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D104">
         <v>92000</v>
       </c>
       <c r="E104" s="1">
         <f t="shared" si="6"/>
-        <v>543.37982249608172</v>
+        <v>543379.8224960817</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" si="8"/>
@@ -2748,14 +2747,14 @@
     <row r="105" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B105" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D105">
         <v>94000</v>
       </c>
       <c r="E105" s="1">
         <f t="shared" si="6"/>
-        <v>531.8205991845515</v>
+        <v>531820.59918455151</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" si="8"/>
@@ -2765,14 +2764,14 @@
     <row r="106" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B106" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D106">
         <v>96000</v>
       </c>
       <c r="E106" s="1">
         <f t="shared" si="6"/>
-        <v>520.74292657533499</v>
+        <v>520742.92657533492</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" si="8"/>
@@ -2782,14 +2781,14 @@
     <row r="107" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B107" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D107">
         <v>98000</v>
       </c>
       <c r="E107" s="1">
         <f t="shared" si="6"/>
-        <v>510.11732698513777</v>
+        <v>510117.32698513777</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="8"/>
@@ -2799,14 +2798,14 @@
     <row r="108" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B108" s="1">
         <f t="shared" si="7"/>
-        <v>3000000</v>
+        <v>3000000000</v>
       </c>
       <c r="D108">
         <v>100000</v>
       </c>
       <c r="E108" s="1">
         <f t="shared" si="6"/>
-        <v>499.91668055326954</v>
+        <v>499916.68055326957</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" si="8"/>

</xml_diff>